<commit_message>
Project Planner for Tomorrow
</commit_message>
<xml_diff>
--- a/Final Summative Project Planner.xlsx
+++ b/Final Summative Project Planner.xlsx
@@ -170,32 +170,12 @@
     <t>QuestionMC Coding - Lily</t>
   </si>
   <si>
-    <t>User Interface Coding - Group</t>
-  </si>
-  <si>
     <t>The Problem Defintion - Group</t>
   </si>
   <si>
     <t>Feature Description - Group</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Resources  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Group</t>
-    </r>
-  </si>
-  <si>
-    <t>Design Touch Ups - Group</t>
-  </si>
-  <si>
     <t>QuestionTF Class Coding - Lily</t>
   </si>
   <si>
@@ -206,12 +186,6 @@
   </si>
   <si>
     <t>Jan.</t>
-  </si>
-  <si>
-    <t>Integrated Testing - Group</t>
-  </si>
-  <si>
-    <t>Software Packaging/Delivery - Group</t>
   </si>
   <si>
     <t>Quiz Class Coding - Janujan</t>
@@ -234,9 +208,6 @@
     </r>
   </si>
   <si>
-    <t>Player Class Design - Pavneet</t>
-  </si>
-  <si>
     <t>Player List Class Design - Kevin</t>
   </si>
   <si>
@@ -264,10 +235,39 @@
     <t>Category Class Coding - Pavneet</t>
   </si>
   <si>
-    <t>Category Class  Design - Lily</t>
-  </si>
-  <si>
     <t>Statistics Class Coding - Pavneet</t>
+  </si>
+  <si>
+    <t>User Interface Coding - Janujan</t>
+  </si>
+  <si>
+    <t>Category Class  Design - Pavneet</t>
+  </si>
+  <si>
+    <t>Design Touch Ups - Janujan</t>
+  </si>
+  <si>
+    <t>Player Class Design - Kevin</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Resources  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Janujan</t>
+    </r>
+  </si>
+  <si>
+    <t>Software Packaging/Delivery - Kevin</t>
+  </si>
+  <si>
+    <t>Integrated Testing - Pavneet</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1099,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="16"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="21"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1127,7 +1127,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1172,7 +1172,7 @@
         <xdr:cNvPr id="2" name="Diamond 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,7 +1232,7 @@
         <xdr:cNvPr id="4" name="Diamond 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1292,7 +1292,7 @@
         <xdr:cNvPr id="5" name="Diamond 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1570,8 +1570,8 @@
   <dimension ref="B2:BQ52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO31" sqref="AO31"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ40" sqref="A1:AJ40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1614,7 +1614,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.3">
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="10" spans="2:69" s="22" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="19">
         <v>2</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="16">
         <v>2</v>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C12" s="16">
         <v>2</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="13" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C13" s="16">
         <v>3</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C14" s="16">
         <v>4</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C15" s="16">
         <v>5</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" s="16">
         <v>5</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C17" s="16">
         <v>5</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C18" s="16">
         <v>5</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" s="16">
         <v>6</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C20" s="16">
         <v>6</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C21" s="16">
         <v>6</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C22" s="16">
         <v>6</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="23" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C23" s="16">
         <v>8</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="24" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="23" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C24" s="16">
         <v>10</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C26" s="16">
         <v>12</v>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C28" s="16">
         <v>12</v>
@@ -2387,7 +2387,7 @@
         <v>18</v>
       </c>
       <c r="F28" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G28" s="17">
         <v>0.9</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C29" s="16">
         <v>12</v>
@@ -2407,10 +2407,10 @@
         <v>13</v>
       </c>
       <c r="F29" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G29" s="17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2424,7 +2424,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F30" s="16">
         <v>3</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C31" s="16">
         <v>15</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C33" s="16">
         <v>18</v>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C34" s="16">
         <v>18</v>
@@ -2507,15 +2507,15 @@
         <v>13</v>
       </c>
       <c r="F34" s="16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G34" s="17">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C35" s="16">
         <v>21</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="37" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C37" s="16">
         <v>24</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="38" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C38" s="16">
         <v>26</v>

</xml_diff>

<commit_message>
Added Read Me file and User Manuel
</commit_message>
<xml_diff>
--- a/Final Summative Project Planner.xlsx
+++ b/Final Summative Project Planner.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Plan</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>QuestionMC Coding - Lily</t>
-  </si>
-  <si>
-    <t>Feature Description - Group</t>
   </si>
   <si>
     <t>QuestionTF Class Coding - Lily</t>
@@ -1102,7 +1099,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="21"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="26"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1130,7 +1127,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1175,7 +1172,7 @@
         <xdr:cNvPr id="2" name="Diamond 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1235,7 +1232,7 @@
         <xdr:cNvPr id="4" name="Diamond 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1295,7 +1292,7 @@
         <xdr:cNvPr id="5" name="Diamond 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1574,7 +1571,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="AH22" sqref="AH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1614,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1660,10 +1657,10 @@
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.3">
       <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -1987,7 +1984,7 @@
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2007,7 +2004,7 @@
     </row>
     <row r="10" spans="2:69" s="22" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="19">
         <v>2</v>
@@ -2048,7 +2045,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="16">
         <v>2</v>
@@ -2068,7 +2065,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="16">
         <v>2</v>
@@ -2088,7 +2085,7 @@
     </row>
     <row r="13" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="16">
         <v>3</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="16">
         <v>4</v>
@@ -2128,7 +2125,7 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="16">
         <v>5</v>
@@ -2148,7 +2145,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="16">
         <v>5</v>
@@ -2168,7 +2165,7 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="16">
         <v>5</v>
@@ -2188,7 +2185,7 @@
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="16">
         <v>5</v>
@@ -2208,7 +2205,7 @@
     </row>
     <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="16">
         <v>6</v>
@@ -2228,7 +2225,7 @@
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="16">
         <v>6</v>
@@ -2248,7 +2245,7 @@
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="16">
         <v>6</v>
@@ -2268,7 +2265,7 @@
     </row>
     <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="16">
         <v>6</v>
@@ -2288,7 +2285,7 @@
     </row>
     <row r="23" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="16">
         <v>8</v>
@@ -2308,7 +2305,7 @@
     </row>
     <row r="24" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="16">
         <v>10</v>
@@ -2338,7 +2335,7 @@
     </row>
     <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="16">
         <v>12</v>
@@ -2378,7 +2375,7 @@
     </row>
     <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="16">
         <v>12</v>
@@ -2398,7 +2395,7 @@
     </row>
     <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="16">
         <v>12</v>
@@ -2413,7 +2410,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2438,7 +2435,7 @@
     </row>
     <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="16">
         <v>15</v>
@@ -2478,7 +2475,7 @@
     </row>
     <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="16">
         <v>18</v>
@@ -2498,7 +2495,7 @@
     </row>
     <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="16">
         <v>18</v>
@@ -2518,7 +2515,7 @@
     </row>
     <row r="35" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="16">
         <v>21</v>
@@ -2548,7 +2545,7 @@
     </row>
     <row r="37" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="16">
         <v>24</v>
@@ -2563,12 +2560,12 @@
         <v>2</v>
       </c>
       <c r="G37" s="17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="16">
         <v>26</v>
@@ -2583,7 +2580,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>